<commit_message>
added roles to the system and judges can now add vacations (short and long)
</commit_message>
<xml_diff>
--- a/DB_DATA/Average_weight_of_case.xlsx
+++ b/DB_DATA/Average_weight_of_case.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/omersamet/Documents/Personal Docs/Google/AlgoLaw/DB_DATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12AF52F4-1BAA-3945-9CBD-245E5430E663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF9AAEB5-A5AA-0B41-BE78-D94F5AB89BF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-100" yWindow="460" windowWidth="23260" windowHeight="12580" xr2:uid="{153EB0C6-CF56-4BAD-BEDB-4FC07FD97B20}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="19760" xr2:uid="{153EB0C6-CF56-4BAD-BEDB-4FC07FD97B20}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -425,7 +426,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>